<commit_message>
bug fixes, added paper, added additional graphs
</commit_message>
<xml_diff>
--- a/graphics.xlsx
+++ b/graphics.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reduced Most Seen" sheetId="6" r:id="rId1"/>
@@ -5605,24 +5605,35 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1025422549155549"/>
+          <c:y val="6.1599396616396358E-2"/>
+          <c:w val="0.87861453729876071"/>
+          <c:h val="0.9179186759966057"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>'Most Seen bygraph'!$A$2:$A$28</c:f>
@@ -5716,7 +5727,7 @@
             <c:numRef>
               <c:f>'Most Seen bygraph'!$E$2:$E$28</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>0.62635280999999998</c:v>
@@ -5758,50 +5769,51 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5151199999999809E-3</c:v>
+                  <c:v>-1.5151199999999809E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0725129999999981E-2</c:v>
+                  <c:v>-2.0725129999999981E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.3409090000000048E-2</c:v>
+                  <c:v>-5.3409090000000048E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9253219999999995E-2</c:v>
+                  <c:v>-5.9253219999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.10725107</c:v>
+                  <c:v>-0.10725107</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.13219694000000004</c:v>
+                  <c:v>-0.13219694000000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.15817099000000001</c:v>
+                  <c:v>-0.15817099000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.19280305999999997</c:v>
+                  <c:v>-0.19280305999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.20757579000000004</c:v>
+                  <c:v>-0.20757579000000004</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.30654760000000003</c:v>
+                  <c:v>-0.30654760000000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.33344157000000002</c:v>
+                  <c:v>-0.33344157000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.37559520000000002</c:v>
+                  <c:v>-0.37559520000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.38160174000000002</c:v>
+                  <c:v>-0.38160174000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.46174239000000006</c:v>
+                  <c:v>-0.46174239000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6537-4502-AE51-AF38FADCC113}"/>
@@ -5816,17 +5828,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
+        <c:smooth val="0"/>
         <c:axId val="348073968"/>
         <c:axId val="348074952"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="348073968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5877,7 +5889,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -5892,7 +5904,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -16302,16 +16314,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>429025</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>68517</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114139</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>4644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>527637</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>158164</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>212751</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>94291</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17961,8 +17973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17997,8 +18009,8 @@
         <f t="shared" ref="D2:D28" si="0">B2-C2</f>
         <v>0.62635280999999998</v>
       </c>
-      <c r="E2">
-        <f>ABS(D2)</f>
+      <c r="E2" s="2">
+        <f>(D2)</f>
         <v>0.62635280999999998</v>
       </c>
     </row>
@@ -18016,8 +18028,8 @@
         <f t="shared" si="0"/>
         <v>0.56103891999999989</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E28" si="1">ABS(D3)</f>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E28" si="1">(D3)</f>
         <v>0.56103891999999989</v>
       </c>
     </row>
@@ -18035,7 +18047,7 @@
         <f t="shared" si="0"/>
         <v>0.35432901</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f t="shared" si="1"/>
         <v>0.35432901</v>
       </c>
@@ -18054,7 +18066,7 @@
         <f t="shared" si="0"/>
         <v>0.25703462999999999</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>0.25703462999999999</v>
       </c>
@@ -18073,7 +18085,7 @@
         <f t="shared" si="0"/>
         <v>0.17348488000000001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
         <v>0.17348488000000001</v>
       </c>
@@ -18092,7 +18104,7 @@
         <f t="shared" si="0"/>
         <v>0.14886363999999996</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>0.14886363999999996</v>
       </c>
@@ -18111,7 +18123,7 @@
         <f t="shared" si="0"/>
         <v>0.14393942999999998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>0.14393942999999998</v>
       </c>
@@ -18130,7 +18142,7 @@
         <f t="shared" si="0"/>
         <v>9.4480490000000028E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>9.4480490000000028E-2</v>
       </c>
@@ -18149,7 +18161,7 @@
         <f t="shared" si="0"/>
         <v>8.0844130000000014E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
         <v>8.0844130000000014E-2</v>
       </c>
@@ -18168,7 +18180,7 @@
         <f t="shared" si="0"/>
         <v>7.6244640000000002E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="1"/>
         <v>7.6244640000000002E-2</v>
       </c>
@@ -18187,7 +18199,7 @@
         <f t="shared" si="0"/>
         <v>4.5995709999999967E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="1"/>
         <v>4.5995709999999967E-2</v>
       </c>
@@ -18206,7 +18218,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -18225,7 +18237,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -18244,9 +18256,9 @@
         <f t="shared" si="0"/>
         <v>-1.5151199999999809E-3</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>1.5151199999999809E-3</v>
+        <v>-1.5151199999999809E-3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -18263,9 +18275,9 @@
         <f t="shared" si="0"/>
         <v>-2.0725129999999981E-2</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>2.0725129999999981E-2</v>
+        <v>-2.0725129999999981E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -18282,9 +18294,9 @@
         <f t="shared" si="0"/>
         <v>-5.3409090000000048E-2</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>5.3409090000000048E-2</v>
+        <v>-5.3409090000000048E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -18301,9 +18313,9 @@
         <f t="shared" si="0"/>
         <v>-5.9253219999999995E-2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>5.9253219999999995E-2</v>
+        <v>-5.9253219999999995E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -18320,9 +18332,9 @@
         <f t="shared" si="0"/>
         <v>-0.10725107</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>0.10725107</v>
+        <v>-0.10725107</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -18339,9 +18351,9 @@
         <f t="shared" si="0"/>
         <v>-0.13219694000000004</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>0.13219694000000004</v>
+        <v>-0.13219694000000004</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -18358,9 +18370,9 @@
         <f t="shared" si="0"/>
         <v>-0.15817099000000001</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <f t="shared" si="1"/>
-        <v>0.15817099000000001</v>
+        <v>-0.15817099000000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -18377,9 +18389,9 @@
         <f t="shared" si="0"/>
         <v>-0.19280305999999997</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f t="shared" si="1"/>
-        <v>0.19280305999999997</v>
+        <v>-0.19280305999999997</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -18396,9 +18408,9 @@
         <f t="shared" si="0"/>
         <v>-0.20757579000000004</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f t="shared" si="1"/>
-        <v>0.20757579000000004</v>
+        <v>-0.20757579000000004</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -18415,9 +18427,9 @@
         <f t="shared" si="0"/>
         <v>-0.30654760000000003</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <f t="shared" si="1"/>
-        <v>0.30654760000000003</v>
+        <v>-0.30654760000000003</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -18434,9 +18446,9 @@
         <f t="shared" si="0"/>
         <v>-0.33344157000000002</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <f t="shared" si="1"/>
-        <v>0.33344157000000002</v>
+        <v>-0.33344157000000002</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -18453,9 +18465,9 @@
         <f t="shared" si="0"/>
         <v>-0.37559520000000002</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <f t="shared" si="1"/>
-        <v>0.37559520000000002</v>
+        <v>-0.37559520000000002</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -18472,9 +18484,9 @@
         <f t="shared" si="0"/>
         <v>-0.38160174000000002</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <f t="shared" si="1"/>
-        <v>0.38160174000000002</v>
+        <v>-0.38160174000000002</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -18491,9 +18503,9 @@
         <f t="shared" si="0"/>
         <v>-0.46174239000000006</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <f t="shared" si="1"/>
-        <v>0.46174239000000006</v>
+        <v>-0.46174239000000006</v>
       </c>
     </row>
     <row r="45" spans="19:19" x14ac:dyDescent="0.3">
@@ -20188,7 +20200,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>

</xml_diff>